<commit_message>
add three more columns
</commit_message>
<xml_diff>
--- a/data/Annual Average Crude Oil Price.xlsx
+++ b/data/Annual Average Crude Oil Price.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kejiawu/DIRECT/Project!/Clean-Energy-Outlook/backup/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicardoZhang\Desktop\project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14660" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14655" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="origin" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Annual Average </t>
   </si>
@@ -56,15 +57,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -78,6 +79,13 @@
       <sz val="16"/>
       <color rgb="FF666666"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="DengXian"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,16 +112,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -382,35 +393,837 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="20.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="20.25">
+      <c r="A2" s="2">
+        <v>1946</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1.63</v>
+      </c>
+      <c r="C2" s="3">
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="20.25">
+      <c r="A3" s="2">
+        <v>1947</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2.16</v>
+      </c>
+      <c r="C3" s="3">
+        <v>23.27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="20.25">
+      <c r="A4" s="2">
+        <v>1948</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2.77</v>
+      </c>
+      <c r="C4" s="3">
+        <v>27.76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="20.25">
+      <c r="A5" s="2">
+        <v>1949</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2.77</v>
+      </c>
+      <c r="C5" s="3">
+        <v>28.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="20.25">
+      <c r="A6" s="2">
+        <v>1950</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2.77</v>
+      </c>
+      <c r="C6" s="3">
+        <v>27.73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="20.25">
+      <c r="A7" s="2">
+        <v>1951</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2.77</v>
+      </c>
+      <c r="C7" s="3">
+        <v>25.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="20.25">
+      <c r="A8" s="2">
+        <v>1952</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2.77</v>
+      </c>
+      <c r="C8" s="3">
+        <v>25.13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="20.25">
+      <c r="A9" s="2">
+        <v>1953</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2.92</v>
+      </c>
+      <c r="C9" s="3">
+        <v>26.23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="20.25">
+      <c r="A10" s="2">
+        <v>1954</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2.99</v>
+      </c>
+      <c r="C10" s="3">
+        <v>26.82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="20.25">
+      <c r="A11" s="2">
+        <v>1955</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2.93</v>
+      </c>
+      <c r="C11" s="3">
+        <v>26.31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="20.25">
+      <c r="A12" s="2">
+        <v>1956</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2.94</v>
+      </c>
+      <c r="C12" s="3">
+        <v>26.07</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="20.25">
+      <c r="A13" s="2">
+        <v>1957</v>
+      </c>
+      <c r="B13" s="3">
+        <v>3.14</v>
+      </c>
+      <c r="C13" s="3">
+        <v>26.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="20.25">
+      <c r="A14" s="2">
+        <v>1958</v>
+      </c>
+      <c r="B14" s="3">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3">
+        <v>25.04</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="20.25">
+      <c r="A15" s="2">
+        <v>1959</v>
+      </c>
+      <c r="B15" s="3">
+        <v>3</v>
+      </c>
+      <c r="C15" s="3">
+        <v>24.79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="20.25">
+      <c r="A16" s="2">
+        <v>1960</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.91</v>
+      </c>
+      <c r="C16" s="3">
+        <v>23.72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="20.25">
+      <c r="A17" s="2">
+        <v>1961</v>
+      </c>
+      <c r="B17" s="3">
+        <v>2.85</v>
+      </c>
+      <c r="C17" s="3">
+        <v>22.96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="20.25">
+      <c r="A18" s="2">
+        <v>1962</v>
+      </c>
+      <c r="B18" s="3">
+        <v>2.85</v>
+      </c>
+      <c r="C18" s="3">
+        <v>22.69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="20.25">
+      <c r="A19" s="2">
+        <v>1963</v>
+      </c>
+      <c r="B19" s="3">
+        <v>2.91</v>
+      </c>
+      <c r="C19" s="3">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="20.25">
+      <c r="A20" s="2">
+        <v>1964</v>
+      </c>
+      <c r="B20" s="3">
+        <v>3</v>
+      </c>
+      <c r="C20" s="3">
+        <v>23.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="20.25">
+      <c r="A21" s="2">
+        <v>1965</v>
+      </c>
+      <c r="B21" s="3">
+        <v>3.01</v>
+      </c>
+      <c r="C21" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="20.25">
+      <c r="A22" s="2">
+        <v>1966</v>
+      </c>
+      <c r="B22" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="C22" s="3">
+        <v>23.01</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="20.25">
+      <c r="A23" s="2">
+        <v>1967</v>
+      </c>
+      <c r="B23" s="3">
+        <v>3.12</v>
+      </c>
+      <c r="C23" s="3">
+        <v>22.53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="20.25">
+      <c r="A24" s="2">
+        <v>1968</v>
+      </c>
+      <c r="B24" s="3">
+        <v>3.18</v>
+      </c>
+      <c r="C24" s="3">
+        <v>21.99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="20.25">
+      <c r="A25" s="2">
+        <v>1969</v>
+      </c>
+      <c r="B25" s="3">
+        <v>3.32</v>
+      </c>
+      <c r="C25" s="3">
+        <v>21.81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="20.25">
+      <c r="A26" s="2">
+        <v>1970</v>
+      </c>
+      <c r="B26" s="3">
+        <v>3.39</v>
+      </c>
+      <c r="C26" s="3">
+        <v>21.04</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="20.25">
+      <c r="A27" s="2">
+        <v>1971</v>
+      </c>
+      <c r="B27" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="C27" s="3">
+        <v>21.42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="20.25">
+      <c r="A28" s="2">
+        <v>1972</v>
+      </c>
+      <c r="B28" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="C28" s="3">
+        <v>20.74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="20.25">
+      <c r="A29" s="2">
+        <v>1973</v>
+      </c>
+      <c r="B29" s="3">
+        <v>4.75</v>
+      </c>
+      <c r="C29" s="3">
+        <v>25.56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="20.25">
+      <c r="A30" s="2">
+        <v>1974</v>
+      </c>
+      <c r="B30" s="3">
+        <v>9.35</v>
+      </c>
+      <c r="C30" s="3">
+        <v>45.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="20.25">
+      <c r="A31" s="2">
+        <v>1975</v>
+      </c>
+      <c r="B31" s="3">
+        <v>12.21</v>
+      </c>
+      <c r="C31" s="3">
+        <v>54.61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="20.25">
+      <c r="A32" s="2">
+        <v>1976</v>
+      </c>
+      <c r="B32" s="3">
+        <v>13.1</v>
+      </c>
+      <c r="C32" s="3">
+        <v>55.46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="20.25">
+      <c r="A33" s="2">
+        <v>1977</v>
+      </c>
+      <c r="B33" s="3">
+        <v>14.4</v>
+      </c>
+      <c r="C33" s="3">
+        <v>57.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="20.25">
+      <c r="A34" s="2">
+        <v>1978</v>
+      </c>
+      <c r="B34" s="3">
+        <v>14.95</v>
+      </c>
+      <c r="C34" s="3">
+        <v>55.24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="20.25">
+      <c r="A35" s="2">
+        <v>1979</v>
+      </c>
+      <c r="B35" s="3">
+        <v>25.1</v>
+      </c>
+      <c r="C35" s="3">
+        <v>82.51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="20.25">
+      <c r="A36" s="2">
+        <v>1980</v>
+      </c>
+      <c r="B36" s="3">
+        <v>37.42</v>
+      </c>
+      <c r="C36" s="3">
+        <v>109.51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="20.25">
+      <c r="A37" s="2">
+        <v>1981</v>
+      </c>
+      <c r="B37" s="3">
+        <v>35.75</v>
+      </c>
+      <c r="C37" s="3">
+        <v>94.83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="20.25">
+      <c r="A38" s="2">
+        <v>1982</v>
+      </c>
+      <c r="B38" s="3">
+        <v>31.83</v>
+      </c>
+      <c r="C38" s="3">
+        <v>79.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="20.25">
+      <c r="A39" s="2">
+        <v>1983</v>
+      </c>
+      <c r="B39" s="3">
+        <v>29.08</v>
+      </c>
+      <c r="C39" s="3">
+        <v>70.34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="20.25">
+      <c r="A40" s="2">
+        <v>1984</v>
+      </c>
+      <c r="B40" s="3">
+        <v>28.75</v>
+      </c>
+      <c r="C40" s="3">
+        <v>66.67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="20.25">
+      <c r="A41" s="2">
+        <v>1985</v>
+      </c>
+      <c r="B41" s="3">
+        <v>26.92</v>
+      </c>
+      <c r="C41" s="3">
+        <v>60.27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="20.25">
+      <c r="A42" s="2">
+        <v>1986</v>
+      </c>
+      <c r="B42" s="3">
+        <v>14.44</v>
+      </c>
+      <c r="C42" s="3">
+        <v>31.72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="20.25">
+      <c r="A43" s="2">
+        <v>1987</v>
+      </c>
+      <c r="B43" s="3">
+        <v>17.75</v>
+      </c>
+      <c r="C43" s="3">
+        <v>37.619999999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="20.25">
+      <c r="A44" s="2">
+        <v>1988</v>
+      </c>
+      <c r="B44" s="3">
+        <v>14.87</v>
+      </c>
+      <c r="C44" s="3">
+        <v>30.33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="20.25">
+      <c r="A45" s="2">
+        <v>1989</v>
+      </c>
+      <c r="B45" s="3">
+        <v>18.329999999999998</v>
+      </c>
+      <c r="C45" s="3">
+        <v>35.6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="20.25">
+      <c r="A46" s="2">
+        <v>1990</v>
+      </c>
+      <c r="B46" s="3">
+        <v>23.19</v>
+      </c>
+      <c r="C46" s="3">
+        <v>42.62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="20.25">
+      <c r="A47" s="2">
+        <v>1991</v>
+      </c>
+      <c r="B47" s="3">
+        <v>20.2</v>
+      </c>
+      <c r="C47" s="3">
+        <v>35.729999999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="20.25">
+      <c r="A48" s="2">
+        <v>1992</v>
+      </c>
+      <c r="B48" s="3">
+        <v>19.25</v>
+      </c>
+      <c r="C48" s="3">
+        <v>33.04</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="20.25">
+      <c r="A49" s="2">
+        <v>1993</v>
+      </c>
+      <c r="B49" s="3">
+        <v>16.75</v>
+      </c>
+      <c r="C49" s="3">
+        <v>27.94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="20.25">
+      <c r="A50" s="2">
+        <v>1994</v>
+      </c>
+      <c r="B50" s="3">
+        <v>15.66</v>
+      </c>
+      <c r="C50" s="3">
+        <v>25.44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="20.25">
+      <c r="A51" s="2">
+        <v>1995</v>
+      </c>
+      <c r="B51" s="3">
+        <v>16.75</v>
+      </c>
+      <c r="C51" s="3">
+        <v>26.48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="20.25">
+      <c r="A52" s="2">
+        <v>1996</v>
+      </c>
+      <c r="B52" s="3">
+        <v>20.46</v>
+      </c>
+      <c r="C52" s="3">
+        <v>31.4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="20.25">
+      <c r="A53" s="2">
+        <v>1997</v>
+      </c>
+      <c r="B53" s="3">
+        <v>18.64</v>
+      </c>
+      <c r="C53" s="3">
+        <v>27.98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="20.25">
+      <c r="A54" s="2">
+        <v>1998</v>
+      </c>
+      <c r="B54" s="3">
+        <v>11.91</v>
+      </c>
+      <c r="C54" s="3">
+        <v>17.600000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="20.25">
+      <c r="A55" s="2">
+        <v>1999</v>
+      </c>
+      <c r="B55" s="3">
+        <v>16.559999999999999</v>
+      </c>
+      <c r="C55" s="3">
+        <v>23.89</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="20.25">
+      <c r="A56" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B56" s="3">
+        <v>27.39</v>
+      </c>
+      <c r="C56" s="3">
+        <v>38.29</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="20.25">
+      <c r="A57" s="2">
+        <v>2001</v>
+      </c>
+      <c r="B57" s="3">
+        <v>23</v>
+      </c>
+      <c r="C57" s="3">
+        <v>31.3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="20.25">
+      <c r="A58" s="2">
+        <v>2002</v>
+      </c>
+      <c r="B58" s="3">
+        <v>22.81</v>
+      </c>
+      <c r="C58" s="3">
+        <v>30.52</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="20.25">
+      <c r="A59" s="2">
+        <v>2003</v>
+      </c>
+      <c r="B59" s="3">
+        <v>27.69</v>
+      </c>
+      <c r="C59" s="3">
+        <v>36.26</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="20.25">
+      <c r="A60" s="2">
+        <v>2004</v>
+      </c>
+      <c r="B60" s="3">
+        <v>37.659999999999997</v>
+      </c>
+      <c r="C60" s="3">
+        <v>47.98</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="20.25">
+      <c r="A61" s="2">
+        <v>2005</v>
+      </c>
+      <c r="B61" s="3">
+        <v>50.04</v>
+      </c>
+      <c r="C61" s="3">
+        <v>61.65</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="20.25">
+      <c r="A62" s="2">
+        <v>2006</v>
+      </c>
+      <c r="B62" s="3">
+        <v>58.3</v>
+      </c>
+      <c r="C62" s="3">
+        <v>69.64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="20.25">
+      <c r="A63" s="2">
+        <v>2007</v>
+      </c>
+      <c r="B63" s="3">
+        <v>64.2</v>
+      </c>
+      <c r="C63" s="3">
+        <v>74.44</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="20.25">
+      <c r="A64" s="2">
+        <v>2008</v>
+      </c>
+      <c r="B64" s="3">
+        <v>91.48</v>
+      </c>
+      <c r="C64" s="3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="20.25">
+      <c r="A65" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B65" s="3">
+        <v>53.48</v>
+      </c>
+      <c r="C65" s="3">
+        <v>59.93</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="20.25">
+      <c r="A66" s="2">
+        <v>2010</v>
+      </c>
+      <c r="B66" s="3">
+        <v>71.209999999999994</v>
+      </c>
+      <c r="C66" s="3">
+        <v>78.650000000000006</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="20.25">
+      <c r="A67" s="2">
+        <v>2011</v>
+      </c>
+      <c r="B67" s="3">
+        <v>87.04</v>
+      </c>
+      <c r="C67" s="3">
+        <v>93.21</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="20.25">
+      <c r="A68" s="2">
+        <v>2012</v>
+      </c>
+      <c r="B68" s="3">
+        <v>86.46</v>
+      </c>
+      <c r="C68" s="3">
+        <v>90.72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="20.25">
+      <c r="A69" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B69" s="3">
+        <v>91.17</v>
+      </c>
+      <c r="C69" s="3">
+        <v>94.25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="20.25">
+      <c r="A70" s="2">
+        <v>2014</v>
+      </c>
+      <c r="B70" s="3">
+        <v>85.6</v>
+      </c>
+      <c r="C70" s="3">
+        <v>87.05</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="20.25">
+      <c r="A71" s="2">
+        <v>2015</v>
+      </c>
+      <c r="B71" s="3">
+        <v>41.85</v>
+      </c>
+      <c r="C71" s="3">
+        <v>42.53</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="20.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="20.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -421,7 +1234,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="20.25">
       <c r="A6" s="2">
         <v>1946</v>
       </c>
@@ -432,7 +1245,7 @@
         <v>19.8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="20.25">
       <c r="A7" s="2">
         <v>1947</v>
       </c>
@@ -443,7 +1256,7 @@
         <v>23.27</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="20.25">
       <c r="A8" s="2">
         <v>1948</v>
       </c>
@@ -454,7 +1267,7 @@
         <v>27.76</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="20.25">
       <c r="A9" s="2">
         <v>1949</v>
       </c>
@@ -465,7 +1278,7 @@
         <v>28.02</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="20.25">
       <c r="A10" s="2">
         <v>1950</v>
       </c>
@@ -476,7 +1289,7 @@
         <v>27.73</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="20.25">
       <c r="A11" s="2">
         <v>1951</v>
       </c>
@@ -487,7 +1300,7 @@
         <v>25.7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="20.25">
       <c r="A12" s="2">
         <v>1952</v>
       </c>
@@ -498,7 +1311,7 @@
         <v>25.13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="20.25">
       <c r="A13" s="2">
         <v>1953</v>
       </c>
@@ -509,7 +1322,7 @@
         <v>26.23</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="20.25">
       <c r="A14" s="2">
         <v>1954</v>
       </c>
@@ -520,7 +1333,7 @@
         <v>26.82</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="20.25">
       <c r="A15" s="2">
         <v>1955</v>
       </c>
@@ -531,7 +1344,7 @@
         <v>26.31</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="20.25">
       <c r="A16" s="2">
         <v>1956</v>
       </c>
@@ -542,7 +1355,7 @@
         <v>26.07</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="20.25">
       <c r="A17" s="2">
         <v>1957</v>
       </c>
@@ -553,7 +1366,7 @@
         <v>26.9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="20.25">
       <c r="A18" s="2">
         <v>1958</v>
       </c>
@@ -564,7 +1377,7 @@
         <v>25.04</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="20.25">
       <c r="A19" s="2">
         <v>1959</v>
       </c>
@@ -575,7 +1388,7 @@
         <v>24.79</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="20.25">
       <c r="A20" s="2">
         <v>1960</v>
       </c>
@@ -586,7 +1399,7 @@
         <v>23.72</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="20.25">
       <c r="A21" s="2">
         <v>1961</v>
       </c>
@@ -597,7 +1410,7 @@
         <v>22.96</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="20.25">
       <c r="A22" s="2">
         <v>1962</v>
       </c>
@@ -608,7 +1421,7 @@
         <v>22.69</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="20.25">
       <c r="A23" s="2">
         <v>1963</v>
       </c>
@@ -619,7 +1432,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="20.25">
       <c r="A24" s="2">
         <v>1964</v>
       </c>
@@ -630,7 +1443,7 @@
         <v>23.3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="20.25">
       <c r="A25" s="2">
         <v>1965</v>
       </c>
@@ -641,7 +1454,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="20.25">
       <c r="A26" s="2">
         <v>1966</v>
       </c>
@@ -652,7 +1465,7 @@
         <v>23.01</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="20.25">
       <c r="A27" s="2">
         <v>1967</v>
       </c>
@@ -663,7 +1476,7 @@
         <v>22.53</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="20.25">
       <c r="A28" s="2">
         <v>1968</v>
       </c>
@@ -674,7 +1487,7 @@
         <v>21.99</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="20.25">
       <c r="A29" s="2">
         <v>1969</v>
       </c>
@@ -685,7 +1498,7 @@
         <v>21.81</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="20.25">
       <c r="A30" s="2">
         <v>1970</v>
       </c>
@@ -696,7 +1509,7 @@
         <v>21.04</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="20.25">
       <c r="A31" s="2">
         <v>1971</v>
       </c>
@@ -707,7 +1520,7 @@
         <v>21.42</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="20.25">
       <c r="A32" s="2">
         <v>1972</v>
       </c>
@@ -718,7 +1531,7 @@
         <v>20.74</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="20.25">
       <c r="A33" s="2">
         <v>1973</v>
       </c>
@@ -729,7 +1542,7 @@
         <v>25.56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="20.25">
       <c r="A34" s="2">
         <v>1974</v>
       </c>
@@ -740,7 +1553,7 @@
         <v>45.6</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="20.25">
       <c r="A35" s="2">
         <v>1975</v>
       </c>
@@ -751,7 +1564,7 @@
         <v>54.61</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="20.25">
       <c r="A36" s="2">
         <v>1976</v>
       </c>
@@ -762,7 +1575,7 @@
         <v>55.46</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="20.25">
       <c r="A37" s="2">
         <v>1977</v>
       </c>
@@ -773,7 +1586,7 @@
         <v>57.2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="20.25">
       <c r="A38" s="2">
         <v>1978</v>
       </c>
@@ -784,7 +1597,7 @@
         <v>55.24</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="20.25">
       <c r="A39" s="2">
         <v>1979</v>
       </c>
@@ -795,7 +1608,7 @@
         <v>82.51</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="20.25">
       <c r="A40" s="2">
         <v>1980</v>
       </c>
@@ -806,7 +1619,7 @@
         <v>109.51</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="20.25">
       <c r="A41" s="2">
         <v>1981</v>
       </c>
@@ -817,7 +1630,7 @@
         <v>94.83</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="20.25">
       <c r="A42" s="2">
         <v>1982</v>
       </c>
@@ -828,7 +1641,7 @@
         <v>79.5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="20.25">
       <c r="A43" s="2">
         <v>1983</v>
       </c>
@@ -839,7 +1652,7 @@
         <v>70.34</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="20.25">
       <c r="A44" s="2">
         <v>1984</v>
       </c>
@@ -850,7 +1663,7 @@
         <v>66.67</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="20.25">
       <c r="A45" s="2">
         <v>1985</v>
       </c>
@@ -861,7 +1674,7 @@
         <v>60.27</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="20.25">
       <c r="A46" s="2">
         <v>1986</v>
       </c>
@@ -872,7 +1685,7 @@
         <v>31.72</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="20.25">
       <c r="A47" s="2">
         <v>1987</v>
       </c>
@@ -883,7 +1696,7 @@
         <v>37.619999999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="20.25">
       <c r="A48" s="2">
         <v>1988</v>
       </c>
@@ -894,7 +1707,7 @@
         <v>30.33</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="20.25">
       <c r="A49" s="2">
         <v>1989</v>
       </c>
@@ -905,7 +1718,7 @@
         <v>35.6</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="20.25">
       <c r="A50" s="2">
         <v>1990</v>
       </c>
@@ -916,7 +1729,7 @@
         <v>42.62</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="20.25">
       <c r="A51" s="2">
         <v>1991</v>
       </c>
@@ -927,7 +1740,7 @@
         <v>35.729999999999997</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="20.25">
       <c r="A52" s="2">
         <v>1992</v>
       </c>
@@ -938,7 +1751,7 @@
         <v>33.04</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="20.25">
       <c r="A53" s="2">
         <v>1993</v>
       </c>
@@ -949,7 +1762,7 @@
         <v>27.94</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="20.25">
       <c r="A54" s="2">
         <v>1994</v>
       </c>
@@ -960,7 +1773,7 @@
         <v>25.44</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="20.25">
       <c r="A55" s="2">
         <v>1995</v>
       </c>
@@ -971,7 +1784,7 @@
         <v>26.48</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="20.25">
       <c r="A56" s="2">
         <v>1996</v>
       </c>
@@ -982,7 +1795,7 @@
         <v>31.4</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="20.25">
       <c r="A57" s="2">
         <v>1997</v>
       </c>
@@ -993,7 +1806,7 @@
         <v>27.98</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="20.25">
       <c r="A58" s="2">
         <v>1998</v>
       </c>
@@ -1004,7 +1817,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="20.25">
       <c r="A59" s="2">
         <v>1999</v>
       </c>
@@ -1015,7 +1828,7 @@
         <v>23.89</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="20.25">
       <c r="A60" s="2">
         <v>2000</v>
       </c>
@@ -1026,7 +1839,7 @@
         <v>38.29</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="20.25">
       <c r="A61" s="2">
         <v>2001</v>
       </c>
@@ -1037,7 +1850,7 @@
         <v>31.3</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="20.25">
       <c r="A62" s="2">
         <v>2002</v>
       </c>
@@ -1048,7 +1861,7 @@
         <v>30.52</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="20.25">
       <c r="A63" s="2">
         <v>2003</v>
       </c>
@@ -1059,7 +1872,7 @@
         <v>36.26</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="20.25">
       <c r="A64" s="2">
         <v>2004</v>
       </c>
@@ -1070,7 +1883,7 @@
         <v>47.98</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="20.25">
       <c r="A65" s="2">
         <v>2005</v>
       </c>
@@ -1081,7 +1894,7 @@
         <v>61.65</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="20.25">
       <c r="A66" s="2">
         <v>2006</v>
       </c>
@@ -1092,7 +1905,7 @@
         <v>69.64</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="20.25">
       <c r="A67" s="2">
         <v>2007</v>
       </c>
@@ -1103,7 +1916,7 @@
         <v>74.44</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" ht="20.25">
       <c r="A68" s="2">
         <v>2008</v>
       </c>
@@ -1114,7 +1927,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="20.25">
       <c r="A69" s="2">
         <v>2009</v>
       </c>
@@ -1125,7 +1938,7 @@
         <v>59.93</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="20.25">
       <c r="A70" s="2">
         <v>2010</v>
       </c>
@@ -1136,7 +1949,7 @@
         <v>78.650000000000006</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="20.25">
       <c r="A71" s="2">
         <v>2011</v>
       </c>
@@ -1147,7 +1960,7 @@
         <v>93.21</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="20.25">
       <c r="A72" s="2">
         <v>2012</v>
       </c>
@@ -1158,7 +1971,7 @@
         <v>90.72</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="20.25">
       <c r="A73" s="2">
         <v>2013</v>
       </c>
@@ -1169,7 +1982,7 @@
         <v>94.25</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="20.25">
       <c r="A74" s="2">
         <v>2014</v>
       </c>
@@ -1180,7 +1993,7 @@
         <v>87.05</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="20.25">
       <c r="A75" s="2">
         <v>2015</v>
       </c>
@@ -1191,7 +2004,7 @@
         <v>42.53</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="20.25">
       <c r="A76" s="2" t="s">
         <v>7</v>
       </c>
@@ -1203,6 +2016,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add oil price in 2016
</commit_message>
<xml_diff>
--- a/data/Annual Average Crude Oil Price.xlsx
+++ b/data/Annual Average Crude Oil Price.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicardoZhang\Desktop\project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicardoZhang\Desktop\project\Clean-Energy-Outlook\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -393,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72:C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1186,6 +1186,17 @@
         <v>42.53</v>
       </c>
     </row>
+    <row r="72" spans="1:3" ht="20.25">
+      <c r="A72" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B72" s="3">
+        <v>34.39</v>
+      </c>
+      <c r="C72" s="3">
+        <v>34.130000000000003</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1197,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76:C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>